<commit_message>
Spreadsheet of JIRA issues and their resolution has been updated during FTF session in Boston Jun 17th.
</commit_message>
<xml_diff>
--- a/Change Control Spreadsheets/Issues in FND and BE.xlsx
+++ b/Change Control Spreadsheets/Issues in FND and BE.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="160" windowWidth="15120" windowHeight="7420" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="15120" windowHeight="7425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FND" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="442">
   <si>
     <t>Target for Dean  and David is 12 June and with MB June 15 in MB regular meeting.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -50,14 +50,6 @@
     <t>Dwiz change to Close no change</t>
   </si>
   <si>
-    <t>Dwiz change to Close no change</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MB to revise definiton.  Dwiz to delay vote</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pete should add this as a JIRA issue</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -846,9 +838,6 @@
     <t>Mike Bennett</t>
   </si>
   <si>
-    <t>Close no change</t>
-  </si>
-  <si>
     <t xml:space="preserve">On reflection, Mike agrees with the riginal model. </t>
   </si>
   <si>
@@ -865,9 +854,6 @@
   </si>
   <si>
     <t>It is currently in Relations - think this is right, since this is used in Group as well as Organization and may be used in other contexts in future. Close no change. The definition may need reviing before we close it. We should also look at ISO 1087 and ISO 11179 and the W3C Organization ontology (for the organizatiojn context of this concept). Need to look into set membership as well; mereology ontologies)</t>
-  </si>
-  <si>
-    <t>Meaning may be more general than just jurisdiction but more specific than Thing, so we still need to fin the middle ground on this one. Also the definition I very specific to Jurisdiction and therefore needs to change. So make the concept and definition match!</t>
   </si>
   <si>
     <t xml:space="preserve">Elisa testing this. This is a 7-bit ASCII character but may be a reserved character somewhere </t>
@@ -1345,13 +1331,60 @@
   </si>
   <si>
     <t>Dwiz change to Close no change.  Added to Ballot #3 20140528</t>
+  </si>
+  <si>
+    <t>Fix no longer moot. All agree on proposed resolution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further discussion 17 June 2014: agreement with the original model is contingent on other changes being made in the way hasCurrency has been used in IND, which would require a separate issue. </t>
+  </si>
+  <si>
+    <t>Redraft the reslolution on this issue</t>
+  </si>
+  <si>
+    <t>to draft</t>
+  </si>
+  <si>
+    <t>FTF Later Resolutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need to summarize in the resolution, what was the argument by which we decided not to change the name of this It's not enough that the raiser agrees to withdraw the issue. 
+The rationale was that we concluded that LegalConstruct as already given was clearer than LegalConferral, even though the possible range of things one might assume form this is broader than the semantics of this term. </t>
+  </si>
+  <si>
+    <t>Meaning may be more general than just jurisdiction but more specific than Thing, so we still need to fin the middle ground on this one. Also the definition is very specific to Jurisdiction and therefore needs to change. So make the concept and definition match!</t>
+  </si>
+  <si>
+    <t>MB to revise definiton.  Dwiz to delay vote. 
+17 Jun further discussions inconclusive: hasMember was intended to be more general than just organizations e.g. set or collection but an organization is not a kind of collection so it may be best to regard this concept fo hasMember as organization-specific after all. Further discussion needed</t>
+  </si>
+  <si>
+    <t>not ready</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is moot in light of #37. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was removed from BCO as part of submission. Consensus is this was correct </t>
+  </si>
+  <si>
+    <t>Jun 17: Remove hasParty and its inverse from the model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hold until we see what Dean and David come up with on lattice treatments. </t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>Need a resolution on this describing the respose we would give to DvK. Also update Section 1 Scope to address these concerns, and mentioninthe response to DvK that this section has been updated in line with his questions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1389,6 +1422,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1410,7 +1449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1430,6 +1469,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1732,7 +1774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1741,922 +1783,922 @@
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="49.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="2" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="2"/>
-    <col min="10" max="10" width="12.5" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="49.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="2"/>
+    <col min="10" max="10" width="12.42578125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="42">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F2" s="2">
         <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="126">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" s="2">
         <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="84">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F5" s="2">
         <v>63</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="28">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="70">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2">
         <v>63</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="56">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="42">
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F13" s="2">
         <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="56">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F14" s="2">
         <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="56">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F15" s="2">
         <v>72</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="56">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F16" s="2">
         <v>89</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="112">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F17" s="2">
         <v>143</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="42">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F18" s="2">
         <v>153</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F19" s="2">
         <v>50</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="70">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F20" s="2">
         <v>97</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="154">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="J21" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="42">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F22" s="2">
         <v>82</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="28">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F23" s="2">
         <v>44</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="112">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="42">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="56">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="D26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="42">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F27" s="2">
         <v>140</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="42">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="84">
+    </row>
+    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="28">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="84">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="84">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="154">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F33" s="2">
         <v>113</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="84">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="70">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2671,155 +2713,155 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28">
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="56">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="56">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="84">
+    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="56">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="70">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2834,1384 +2876,1413 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="26.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="28">
+        <v>247</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>427</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="42">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="42">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="42">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="84">
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="126">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="56">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="70">
+    <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>266</v>
+        <v>428</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>49</v>
+        <v>430</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="70">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="98">
+        <v>430</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>435</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="56">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>273</v>
+        <v>433</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="42">
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="70">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="70">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>49</v>
+        <v>430</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="70">
+        <v>426</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28">
+        <v>426</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="98">
+      <c r="G39" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28">
+        <v>426</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28">
+        <v>392</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>0</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="56">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="42">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="252">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="28">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="126">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="84">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="84">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="84">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="84">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="126">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="84">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="42">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="56">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>63</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="42">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>49</v>
+        <v>430</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="42">
+        <v>41</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>67</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="84">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="28">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="98">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="42">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4221,272 +4292,272 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" customWidth="1"/>
-    <col min="2" max="2" width="50.5" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="6" t="s">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
-      <c r="A4" s="6" t="s">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
-      <c r="A5" s="6" t="s">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
-      <c r="A6" s="6" t="s">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="6" t="s">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="6" t="s">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15">
-      <c r="A9" s="6" t="s">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15">
-      <c r="A10" s="6" t="s">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
-      <c r="A11" s="6" t="s">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
-      <c r="A12" s="6" t="s">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="6" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
-      <c r="A14" s="6" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
-      <c r="A15" s="6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
-      <c r="A16" s="6" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15">
-      <c r="A18" s="6" t="s">
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15">
-      <c r="A19" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15">
-      <c r="A20" s="6" t="s">
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15">
-      <c r="A21" s="6" t="s">
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15">
-      <c r="A22" s="6" t="s">
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15">
-      <c r="A23" s="6" t="s">
+    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15">
-      <c r="A24" s="6" t="s">
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15">
-      <c r="A25" s="6" t="s">
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15">
-      <c r="A26" s="6" t="s">
+    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15">
-      <c r="A27" s="6" t="s">
+    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15">
-      <c r="A28" s="6" t="s">
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15">
-      <c r="A29" s="6" t="s">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15">
-      <c r="A30" s="6" t="s">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15">
-      <c r="A31" s="6" t="s">
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15">
-      <c r="A32" s="6" t="s">
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15">
-      <c r="A33" s="6" t="s">
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15">
-      <c r="A34" s="6" t="s">
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15">
-      <c r="A35" s="6" t="s">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15">
-      <c r="A36" s="6" t="s">
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15">
-      <c r="A37" s="6" t="s">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15">
-      <c r="A38" s="6" t="s">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15">
-      <c r="A39" s="6" t="s">
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15">
-      <c r="A40" s="6" t="s">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15">
-      <c r="A41" s="6" t="s">
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15">
-      <c r="A42" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15">
-      <c r="A43" s="6" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="15">
-      <c r="A44" s="6" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="15">
-      <c r="A45" s="6" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="15">
+    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15">
-      <c r="A47" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="15">
-      <c r="A48" s="6" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15">
-      <c r="A49" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15">
-      <c r="A50" s="6" t="s">
-        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the preadsheet Issues in FND and BE with status of definition issues; added new spreadsheet DefinitionIssuesResolutions detailing the proposed resolutions both as document edits to the specification and as model changes to the source models.
</commit_message>
<xml_diff>
--- a/Change Control Spreadsheets/Issues in FND and BE.xlsx
+++ b/Change Control Spreadsheets/Issues in FND and BE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="15120" windowHeight="7425" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5640" windowWidth="19200" windowHeight="6630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FND" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FND!$A$1:$K$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'JIRA Issues Notes'!$A$1:$G$75</definedName>
   </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="443">
   <si>
     <t>Target for Dean  and David is 12 June and with MB June 15 in MB regular meeting.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1378,6 +1379,9 @@
   </si>
   <si>
     <t>Need a resolution on this describing the respose we would give to DvK. Also update Section 1 Scope to address these concerns, and mentioninthe response to DvK that this section has been updated in line with his questions.</t>
+  </si>
+  <si>
+    <t>Resolution proposed</t>
   </si>
 </sst>
 </file>
@@ -1415,6 +1419,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2879,9 +2884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3186,7 +3191,7 @@
         <v>266</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3348,10 +3353,10 @@
         <v>277</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3365,10 +3370,10 @@
         <v>278</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3382,7 +3387,7 @@
         <v>280</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,7 +3404,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3413,10 +3418,10 @@
         <v>282</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>282</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3447,7 +3452,7 @@
         <v>282</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3481,10 +3486,10 @@
         <v>288</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>289</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3521,7 +3526,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3535,7 +3540,7 @@
         <v>251</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3798,7 +3803,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -3812,10 +3817,10 @@
         <v>295</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -3829,10 +3834,10 @@
         <v>295</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -3846,7 +3851,7 @@
         <v>295</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -4063,7 +4068,7 @@
         <v>310</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>219</v>
+        <v>442</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Proposed material for next ballot. Changes made to proposed definitions during FTF call on 22 July (JIRA #61 and #127); JIRA # 42, 43, 44 taken off the ballot.
No additional comments or corrections received to definitions in JIRA #61 or #127 by the agreed midnight EDT deadline.

The "Almosts" that are flagged as "Resolution Proposed" in the main worksheet are now ready for ballot.
</commit_message>
<xml_diff>
--- a/Change Control Spreadsheets/Issues in FND and BE.xlsx
+++ b/Change Control Spreadsheets/Issues in FND and BE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5760" windowWidth="19200" windowHeight="6510" tabRatio="857" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5760" windowWidth="19200" windowHeight="2085" tabRatio="857" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FND Pre" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="1165">
   <si>
     <t>Target for Dean  and David is 12 June and with MB June 15 in MB regular meeting.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -3780,6 +3780,27 @@
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: for isAssetOf we discussed the resolution on 22 July. Domain should be PartyInRole and range should be ThingInRole once that is added. </t>
+  </si>
+  <si>
+    <t>a person who has attained the age of majority as defined by given jurisdiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a minor who is allowed to conduct a business or any other occupation on his or her own behalf or for their own account outside the control of a parent or guardian. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">any document which may be used to verify aspects of a person's identity. </t>
+  </si>
+  <si>
+    <t>a person under a certain age, usually the age of majority in a given jurisdiction, which legally demarcates childhood from adulthood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a number or text which appears on an identity document issued by a country or jurisdiction.  </t>
+  </si>
+  <si>
+    <t>Resolution Under Review</t>
   </si>
 </sst>
 </file>
@@ -3873,7 +3894,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3931,6 +3952,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3997,7 +4024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4142,6 +4169,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4196,10 +4229,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5986,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6008,27 +6038,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -6152,31 +6182,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56" t="s">
         <v>1046</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="58" t="s">
+      <c r="L1" s="56"/>
+      <c r="M1" s="60" t="s">
         <v>370</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -6348,38 +6378,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="60" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62" t="s">
         <v>1018</v>
       </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="63" t="s">
         <v>556</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63" t="s">
+      <c r="J1" s="64"/>
+      <c r="K1" s="65" t="s">
         <v>557</v>
       </c>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="66" t="s">
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="68" t="s">
         <v>558</v>
       </c>
-      <c r="V1" s="67"/>
+      <c r="V1" s="69"/>
     </row>
     <row r="2" spans="1:22" s="24" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -7212,9 +7242,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7239,10 +7269,10 @@
       <c r="B1" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="70" t="s">
         <v>711</v>
       </c>
-      <c r="D1" s="69"/>
+      <c r="D1" s="71"/>
       <c r="E1" s="36" t="s">
         <v>414</v>
       </c>
@@ -7309,7 +7339,7 @@
         <v>460</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>461</v>
+        <v>1159</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>462</v>
@@ -7358,7 +7388,7 @@
         <v>467</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>468</v>
+        <v>1160</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>469</v>
@@ -7381,7 +7411,7 @@
         <v>470</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>471</v>
+        <v>1161</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>472</v>
@@ -7430,7 +7460,7 @@
         <v>476</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>477</v>
+        <v>1162</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>478</v>
@@ -7453,7 +7483,7 @@
         <v>479</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>480</v>
+        <v>1163</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>479</v>
@@ -7526,10 +7556,10 @@
       <c r="C1" s="34" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="70" t="s">
         <v>711</v>
       </c>
-      <c r="E1" s="69"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="36" t="s">
         <v>414</v>
       </c>
@@ -8296,8 +8326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8795,10 +8825,10 @@
       <c r="C1" s="34" t="s">
         <v>1017</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="70" t="s">
         <v>711</v>
       </c>
-      <c r="E1" s="69"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="36" t="s">
         <v>414</v>
       </c>
@@ -11380,8 +11410,8 @@
   <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12349,8 +12379,8 @@
       <c r="E43" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F43" s="43" t="s">
-        <v>1033</v>
+      <c r="F43" s="72" t="s">
+        <v>1164</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -12369,8 +12399,8 @@
       <c r="E44" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="F44" s="43" t="s">
-        <v>1033</v>
+      <c r="F44" s="72" t="s">
+        <v>1164</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -12386,11 +12416,11 @@
       <c r="D45" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E45" s="70" t="s">
+      <c r="E45" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="F45" s="43" t="s">
-        <v>1033</v>
+      <c r="F45" s="72" t="s">
+        <v>1164</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -12817,7 +12847,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="44">
         <v>62</v>
       </c>
@@ -12835,6 +12865,9 @@
       </c>
       <c r="F65" s="2" t="s">
         <v>219</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>1158</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -13907,13 +13940,13 @@
     <hyperlink ref="A153" r:id="rId150" display="http://solitaire.omg.org/browse/FIBOFTF-149?filter=-4&amp;jql=project%20%3D%20FIBOFTF%20ORDER%20BY%20createdDate%20DESC"/>
     <hyperlink ref="A154" r:id="rId151" display="http://solitaire.omg.org/browse/FIBOFTF-150?filter=-4&amp;jql=project%20%3D%20FIBOFTF%20ORDER%20BY%20createdDate%20DESC"/>
     <hyperlink ref="F43" location="'FND-FTF #42'!A3" display="Resolution Proposed"/>
-    <hyperlink ref="F44" location="'FND-FTF #43'!A3" display="Resolution Proposed"/>
-    <hyperlink ref="F45" location="'FND-FTF #44'!A3" display="Resolution Proposed"/>
     <hyperlink ref="F21" location="'FND-FTF #20'!A3" display="Resolution Proposed"/>
     <hyperlink ref="F28" location="'FND-FTF #27'!A3" display="Resolution Proposed"/>
     <hyperlink ref="F32" location="'FND-FTF #31'!A3" display="Resolution Proposed"/>
     <hyperlink ref="F53" location="'FND-FTF #51'!A3" display="Resolution Proposed"/>
     <hyperlink ref="F75" location="'FND-FTF #72'!A3" display="Resolution Proposed"/>
+    <hyperlink ref="F44" location="'FND-FTF #42'!A3" display="Resolution Proposed"/>
+    <hyperlink ref="F45" location="'FND-FTF #42'!A3" display="Resolution Proposed"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId152"/>
@@ -13932,7 +13965,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14380,7 +14413,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>72</v>
       </c>
@@ -14430,8 +14463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14452,27 +14485,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -14589,27 +14622,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -14717,8 +14750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14739,27 +14772,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -14891,8 +14924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14914,32 +14947,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56" t="s">
         <v>1080</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="55" t="s">
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -15076,7 +15109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -15098,27 +15131,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -15192,7 +15225,7 @@
       <c r="J3" s="2" t="s">
         <v>1085</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="K3" s="53" t="s">
         <v>297</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -15216,7 +15249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="D10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -15238,27 +15271,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>1019</v>
       </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55" t="s">
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -15332,7 +15365,7 @@
       <c r="J3" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="52" t="s">
         <v>296</v>
       </c>
       <c r="L3" s="2" t="s">

</xml_diff>

<commit_message>
Revert "Get the OMG Submission folder"
</commit_message>
<xml_diff>
--- a/Change Control Spreadsheets/Issues in FND and BE.xlsx
+++ b/Change Control Spreadsheets/Issues in FND and BE.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="15120" windowHeight="7425" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="160" windowWidth="15120" windowHeight="7420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FND" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="431">
   <si>
     <t>Target for Dean  and David is 12 June and with MB June 15 in MB regular meeting.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -50,6 +50,14 @@
     <t>Dwiz change to Close no change</t>
   </si>
   <si>
+    <t>Dwiz change to Close no change</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MB to revise definiton.  Dwiz to delay vote</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Pete should add this as a JIRA issue</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -838,6 +846,9 @@
     <t>Mike Bennett</t>
   </si>
   <si>
+    <t>Close no change</t>
+  </si>
+  <si>
     <t xml:space="preserve">On reflection, Mike agrees with the riginal model. </t>
   </si>
   <si>
@@ -854,6 +865,9 @@
   </si>
   <si>
     <t>It is currently in Relations - think this is right, since this is used in Group as well as Organization and may be used in other contexts in future. Close no change. The definition may need reviing before we close it. We should also look at ISO 1087 and ISO 11179 and the W3C Organization ontology (for the organizatiojn context of this concept). Need to look into set membership as well; mereology ontologies)</t>
+  </si>
+  <si>
+    <t>Meaning may be more general than just jurisdiction but more specific than Thing, so we still need to fin the middle ground on this one. Also the definition I very specific to Jurisdiction and therefore needs to change. So make the concept and definition match!</t>
   </si>
   <si>
     <t xml:space="preserve">Elisa testing this. This is a 7-bit ASCII character but may be a reserved character somewhere </t>
@@ -1331,60 +1345,13 @@
   </si>
   <si>
     <t>Dwiz change to Close no change.  Added to Ballot #3 20140528</t>
-  </si>
-  <si>
-    <t>Fix no longer moot. All agree on proposed resolution.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further discussion 17 June 2014: agreement with the original model is contingent on other changes being made in the way hasCurrency has been used in IND, which would require a separate issue. </t>
-  </si>
-  <si>
-    <t>Redraft the reslolution on this issue</t>
-  </si>
-  <si>
-    <t>to draft</t>
-  </si>
-  <si>
-    <t>FTF Later Resolutions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We need to summarize in the resolution, what was the argument by which we decided not to change the name of this It's not enough that the raiser agrees to withdraw the issue. 
-The rationale was that we concluded that LegalConstruct as already given was clearer than LegalConferral, even though the possible range of things one might assume form this is broader than the semantics of this term. </t>
-  </si>
-  <si>
-    <t>Meaning may be more general than just jurisdiction but more specific than Thing, so we still need to fin the middle ground on this one. Also the definition is very specific to Jurisdiction and therefore needs to change. So make the concept and definition match!</t>
-  </si>
-  <si>
-    <t>MB to revise definiton.  Dwiz to delay vote. 
-17 Jun further discussions inconclusive: hasMember was intended to be more general than just organizations e.g. set or collection but an organization is not a kind of collection so it may be best to regard this concept fo hasMember as organization-specific after all. Further discussion needed</t>
-  </si>
-  <si>
-    <t>not ready</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is moot in light of #37. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was removed from BCO as part of submission. Consensus is this was correct </t>
-  </si>
-  <si>
-    <t>Jun 17: Remove hasParty and its inverse from the model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hold until we see what Dean and David come up with on lattice treatments. </t>
-  </si>
-  <si>
-    <t>No change</t>
-  </si>
-  <si>
-    <t>Need a resolution on this describing the respose we would give to DvK. Also update Section 1 Scope to address these concerns, and mentioninthe response to DvK that this section has been updated in line with his questions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1422,12 +1389,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1449,7 +1410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1469,9 +1430,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1774,7 +1732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1783,922 +1741,922 @@
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="49.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" style="2"/>
-    <col min="10" max="10" width="12.42578125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="49.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="2" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="2"/>
+    <col min="10" max="10" width="12.5" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="42">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="2">
         <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="126">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2">
         <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="84">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2">
         <v>63</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="70">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F8" s="2">
         <v>63</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="56">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="42">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F13" s="2">
         <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="56">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="F14" s="2">
         <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="56">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F15" s="2">
         <v>72</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="56">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F16" s="2">
         <v>89</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="112">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F17" s="2">
         <v>143</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="42">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F18" s="2">
         <v>153</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F19" s="2">
         <v>50</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="70">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F20" s="2">
         <v>97</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="154">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="42">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F22" s="2">
         <v>82</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F23" s="2">
         <v>44</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="112">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="42">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="56">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="42">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F27" s="2">
         <v>140</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="42">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="84">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="84">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="84">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="154">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F33" s="2">
         <v>113</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="84">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="70">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2713,155 +2671,155 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="56">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="56">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="84">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="56">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="70">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2876,1413 +2834,1384 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="26.1640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>230</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="84">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="126">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="56">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="70">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>428</v>
+        <v>266</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>430</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="70">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="98">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>435</v>
+        <v>49</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="56">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>433</v>
+        <v>273</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="70">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="70">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" ht="70">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" ht="98">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28">
       <c r="A46" s="2">
         <v>0</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="42">
       <c r="A47" s="2">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="42">
       <c r="A48" s="2">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="56">
       <c r="A49" s="2">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="42">
       <c r="A54" s="2">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="252">
       <c r="A55" s="2">
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="28">
       <c r="A56" s="2">
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="126">
       <c r="A57" s="2">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="84">
       <c r="A58" s="2">
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="84">
       <c r="A59" s="2">
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="84">
       <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F60" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="84">
+      <c r="A61" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="C61" s="2" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="126">
       <c r="A62" s="2">
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="84">
       <c r="A64" s="2">
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="42">
       <c r="A65" s="2">
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="56">
       <c r="A66" s="2">
         <v>63</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28">
       <c r="A67" s="2">
         <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28">
       <c r="A68" s="2">
         <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="42">
       <c r="A69" s="2">
         <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>430</v>
+        <v>49</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="42">
       <c r="A70" s="2">
         <v>67</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="84">
       <c r="A71" s="2">
         <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="28">
       <c r="A72" s="2">
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="98">
       <c r="A73" s="2">
         <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="42">
       <c r="A74" s="2">
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28">
       <c r="A75" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4292,272 +4221,272 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.1640625" customWidth="1"/>
+    <col min="2" max="2" width="50.5" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15">
+      <c r="A17" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15">
+      <c r="A18" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15">
+      <c r="A19" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15">
+      <c r="A20" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15">
+      <c r="A21" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15">
+      <c r="A22" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15">
+      <c r="A23" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15">
+      <c r="A24" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15">
+      <c r="A25" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15">
+      <c r="A26" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15">
+      <c r="A27" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15">
+      <c r="A28" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15">
+      <c r="A29" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15">
+      <c r="A30" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15">
+      <c r="A31" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15">
+      <c r="A32" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15">
+      <c r="A33" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15">
+      <c r="A34" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15">
+      <c r="A35" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15">
+      <c r="A36" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15">
+      <c r="A37" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15">
+      <c r="A38" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15">
+      <c r="A39" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15">
+      <c r="A40" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15">
+      <c r="A41" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15">
+      <c r="A42" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15">
+      <c r="A43" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15">
+      <c r="A44" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15">
+      <c r="A45" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15">
+      <c r="A46" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15">
+      <c r="A47" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="7" t="s">
+    </row>
+    <row r="48" spans="1:1" ht="15">
+      <c r="A48" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15">
+      <c r="A49" s="6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="15">
       <c r="A50" s="6" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>